<commit_message>
Update import user for livestream
</commit_message>
<xml_diff>
--- a/src/static/files/statsUser_template.xlsx
+++ b/src/static/files/statsUser_template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\py\DJ_Project\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\py\DJ_Project\src\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB59687D-EE16-450D-A8B3-0986784D11A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AF3979-8533-4B63-B959-793B04C47B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4515" yWindow="4125" windowWidth="14280" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>khach_hang</t>
-  </si>
-  <si>
     <t>TN010</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>so_tem</t>
+  </si>
+  <si>
+    <t>maKH</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -380,18 +380,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -402,7 +402,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>11</v>
@@ -413,7 +413,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -424,7 +424,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>13</v>
@@ -435,7 +435,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>14</v>

</xml_diff>